<commit_message>
msl40v1 - update taxonomy
also fix older test cases for new, better, species name filters (change some spaces to dashes, to avoid errors we don't want)

Switching over to versions based on msl##v#, instead of v#.#. Much more informative.
</commit_message>
<xml_diff>
--- a/testData/msl38/proposalsMultiFileLinking/2023.10M.N.v1.CreateSpeciesFirst.xlsx
+++ b/testData/msl38/proposalsMultiFileLinking/2023.10M.N.v1.CreateSpeciesFirst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/validate_proposals/testData/proposalsMultiFileLinking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/load_msl/testData/msl38/proposalsMultiFileLinking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610FB13C-F93D-ED4B-895D-7B04B3B42ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DF1419-1875-1549-BCB3-C4309DC9B91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6200" windowWidth="34560" windowHeight="15840" activeTab="1" xr2:uid="{94A59F7B-7A42-3941-BED7-E7ACB004C4FA}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="29920" windowHeight="15840" activeTab="1" xr2:uid="{94A59F7B-7A42-3941-BED7-E7ACB004C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -1664,9 +1664,6 @@
     <t>GenusCreatedLater20Virus</t>
   </si>
   <si>
-    <t>GenusCreatedLater20Virus Species10 Two and Three</t>
-  </si>
-  <si>
     <t>GenusCreatedLater20Virus Species10</t>
   </si>
   <si>
@@ -1692,6 +1689,9 @@
   </si>
   <si>
     <t>Species10to30to20</t>
+  </si>
+  <si>
+    <t>GenusCreatedLater20Virus Species10-Two-and-Three</t>
   </si>
 </sst>
 </file>
@@ -2277,9 +2277,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2317,7 +2317,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2423,7 +2423,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2565,7 +2565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2607,9 +2607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2286CF-D255-A24B-BEAA-53A574258AAC}">
   <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF11" sqref="Z11:AF11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2950,13 +2950,13 @@
       <c r="V5" s="35"/>
       <c r="X5" s="36"/>
       <c r="Z5" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB5" s="14" t="s">
         <v>121</v>
       </c>
       <c r="AD5" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AK5" s="4" t="s">
         <v>63</v>
@@ -2973,13 +2973,13 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z6" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB6" s="14" t="s">
         <v>121</v>
       </c>
       <c r="AD6" s="26" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="AK6" s="4" t="s">
         <v>63</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z7" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB7" s="14" t="s">
         <v>120</v>
@@ -3013,13 +3013,13 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z8" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB8" s="14" t="s">
         <v>120</v>
       </c>
       <c r="AD8" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AK8" s="4" t="s">
         <v>63</v>
@@ -3036,13 +3036,13 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z9" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB9" s="14" t="s">
         <v>120</v>
       </c>
       <c r="AD9" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AK9" s="4" t="s">
         <v>63</v>
@@ -3059,10 +3059,10 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB10" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="AB10" s="14" t="s">
-        <v>127</v>
       </c>
       <c r="AL10" s="15" t="s">
         <v>27</v>
@@ -3071,21 +3071,21 @@
         <v>35</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="Z11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB11" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="AB11" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="AD11" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="AK11" s="4" t="s">
         <v>98</v>
@@ -3097,7 +3097,7 @@
         <v>28</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -3178,8 +3178,8 @@
       <formula>NOT(AM4=proposedRank)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="22">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD4" xr:uid="{C3BFCEE8-5F4E-4218-B34F-5F2909915D3E}">
+  <dataValidations count="17">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD4 AD14:AD17 AD19:AD20 AD27" xr:uid="{C3BFCEE8-5F4E-4218-B34F-5F2909915D3E}">
       <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD31:AD1048576 AD22" xr:uid="{77DCB41F-881F-4ED8-B4E4-952B298D5F1E}">
@@ -3187,9 +3187,6 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD1:AD3 AD5:AD6" xr:uid="{C41C12C6-6B99-41E7-9220-B018159F2448}">
       <formula1>OR(LEFT(AD1048575,LEN(AB1048575))=AB1048575,AD1048575="Species")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD19:AD20 AD27" xr:uid="{E99188F1-7165-4849-AEC6-40F8A78582FB}">
-      <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" errorTitle="No spaces allowed" error="Taxon names above the rank of species may NOT contain spaces." promptTitle="No spaces allowed" prompt="Taxon names above the rank of species may NOT contain spaces." sqref="P1:P4 Q3:AC4 P5:AC1048576" xr:uid="{52FC0539-8CE1-4D6A-8AE9-C667226BA6D9}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD23 AD9" xr:uid="{FB4AE646-A3B6-45D8-989E-CE736059B2BA}">
@@ -3213,9 +3210,6 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD15" xr:uid="{E94EB4B0-749B-4F68-9541-D7546586CB32}">
       <formula1>OR(LEFT(AD26,LEN(AB26))=AB26,AD26="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD14" xr:uid="{B0E4334B-E48E-429C-89DA-1B72B252BF95}">
-      <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD8" xr:uid="{9A862997-BEDA-40BD-A38E-553D82982759}">
       <formula1>OR(LEFT(AD17,LEN(AB17))=AB17,AD17="Species")</formula1>
     </dataValidation>
@@ -3230,15 +3224,6 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD18" xr:uid="{58B13D35-BB13-4805-9934-45C7671A030E}">
       <formula1>OR(LEFT(AD8,LEN(AB8))=AB8,AD8="Species")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD17" xr:uid="{0339AE28-7906-4A43-99EB-486A28435F1E}">
-      <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD16" xr:uid="{7103EC30-1786-4FAE-8A86-96EE531A7CA1}">
-      <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD15" xr:uid="{E8BF44B8-49C7-4650-BD5B-04B37AD54A3E}">
-      <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="AD14" xr:uid="{67710291-D695-4D15-8134-AED9C429D1B9}">
       <formula1>OR(LEFT(AD20,LEN(AB20))=AB20,AD20="Species")</formula1>

</xml_diff>